<commit_message>
tickers terminados Relatorio e Media faltando
</commit_message>
<xml_diff>
--- a/codes/database/Produto.xlsx
+++ b/codes/database/Produto.xlsx
@@ -463,19 +463,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">O mercado de debêntures incentivadas, títulos de renda fixa isentos de imposto de renda, está em alta. Impulsionado pelo boom da renda fixa e pelas restrições a outros títulos isentos, como LCIs e LCAs, o volume de emissões saltou 385% desde 2019, atingindo R$ 77,78 bilhões no primeiro semestre de 2024.
-Emitidas por empresas para financiar projetos de infraestrutura, as debêntures incentivadas atraem investidores em busca de retornos maiores e diversificação. Entre os principais emissores, destacam-se Petrobras, Rumo, Eneva, Engie e CCR, com ofertas que podem ultrapassar R$ 9 bilhões. 
+          <t xml:space="preserve">O mercado de debêntures incentivadas, títulos de renda fixa isentos de imposto de renda, está em alta, impulsionado pelo boom da renda fixa e pelas restrições a outros títulos isentos. Essas debêntures, emitidas por empresas para financiar projetos de infraestrutura, tiveram um salto de 385% em emissões entre o primeiro semestre de 2019 e 2024, atingindo R$ 77,78 bilhões. A migração de investidores de LCIs, LCAs, CRIs e CRAs, devido a limites impostos pelo governo, contribuiu para o crescimento do mercado. As debêntures incentivadas tornaram-se atrativas por seu potencial de retorno e como alternativa de diversificação. Entre os principais emissores estão empresas como Petrobras, Rumo, Eneva e Engie. 
 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>O, CCR, R</t>
+          <t xml:space="preserve">- PETR4
+- RAIL3
+- ENEV3
+- EGIE3
+- CCRO3 
+</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>negative (74.86000061035156%)</t>
+          <t>negative (80.87999725341797%)</t>
         </is>
       </c>
     </row>
@@ -487,18 +491,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">A Rivool Finance lança braço de banco de investimento liderado por Fernando Fegyveres, ex-CEO do Voiter e agora sócio da fintech. A iniciativa expande a atuação da empresa, que conecta investidores do Brasil e do exterior ao mercado de crédito nacional através da tokenização, simplificando o acesso a esse tipo de investimento. A chegada de Fegyveres e a criação do braço de investimentos demonstram a ambição da Rivool em consolidar sua posição nesse mercado em crescimento. 
+          <t xml:space="preserve">A Rivool Finance lança braço de banco de investimento liderado por Fernando Fegyveres, ex-CEO do Voiter e agora sócio da fintech. A iniciativa amplia a atuação da empresa que conecta investidores do Brasil e do exterior ao mercado de crédito nacional através da tokenização. A novidade promete abrir novas oportunidades para investidores e fortalecer a presença da Rivool no mercado financeiro.  
 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>A, CEO</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>negative (85.80999755859375%)</t>
+          <t>negative (88.31999969482422%)</t>
         </is>
       </c>
     </row>
@@ -510,18 +515,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Roberto Campos Neto, presidente do Banco Central, anunciou que o Pix por aproximação, via carteira digital do Google, estará disponível em breve. A parceria permitirá o pagamento com Pix por meio de smartphones Android, com roteamento para diversas contas. O BC está aberto a novas parcerias. Campos Neto destacou o avanço da tokenização da economia e mencionou o Pix, a internacionalização da moeda, o Open Finance e o Drex como pilares dessa transformação. Ele ainda apontou a inteligência artificial e a monetização de dados como próximos passos, defendendo que as pessoas deveriam ser remuneradas por seus dados. 
+          <t xml:space="preserve">Roberto Campos Neto, presidente do Banco Central, anunciou que o Pix por aproximação, via carteira digital do Google, estará disponível em breve. A parceria permitirá o pagamento por aproximação utilizando o Pix como método de pagamento, com a opção de roteamento para diferentes contas. Campos Neto ressaltou o avanço da tokenização da economia e apresentou a agenda de tecnologia do BC, incluindo o Pix, internacionalização da moeda, Open Finance e Drex. Ele mencionou ainda a inteligência artificial e a monetização de dados como próximos passos, destacando a importância da remuneração pela cessão de dados. 
 </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>A, O, BC</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>positive (66.69999694824219%)</t>
+          <t>positive (76.51000213623047%)</t>
         </is>
       </c>
     </row>
@@ -533,18 +539,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Roberto Campos Neto, presidente do Banco Central, afirmou que a economia caminha para a tokenização, processo de converter valor em tokens digitais. Ele destacou o Pix, Open Finance e o Drex como exemplos da agenda tecnológica do BC. Campos Neto defende a tokenização e se diz contrário à proibição de ativos virtuais, posição minoritária entre os BCs. Ele acredita que a proibição aumenta os riscos e observa o crescimento das stablecoins como uma busca por alternativas mais baratas para ter conta em dólar. 
+          <t xml:space="preserve">Roberto Campos Neto, presidente do Banco Central, afirmou que a economia caminha para a tokenização, processo de converter ativos em tokens digitais. Ele destacou a tokenização como parte de sua gestão no BC, junto com Pix, Open Finance e Drex. Campos Neto defendeu a posição do BC contra a proibição de ativos virtuais, argumentando que a restrição aumenta o risco. Ele observou que o crescimento se concentra em stablecoins, atreladas a moedas como o dólar, o que pode indicar a busca por alternativas mais baratas para contas em moeda estrangeira. 
 </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>positive (84.69000244140625%)</t>
+          <t>positive (75.55999755859375%)</t>
         </is>
       </c>
     </row>
@@ -556,18 +563,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Roberto Campos Neto, presidente do Banco Central, revelou que o Pix custa US$ 10 milhões/ano para operar, com pico de 240 milhões de transações/dia. O custo inicial, de US$ 3 a 4 milhões, foi dividido com bancos. Campos Neto destacou o sucesso do Pix como porta de entrada para a inovação, abrindo caminho para tokenização, Open Finance e Drex (real digital). Ele prevê a criação de agregadores financeiros unindo essas tecnologias.  O desafio do Drex é escalar com privacidade, programabilidade e descentralização. Soluções em desenvolvimento buscam aumentar o número de transações, ainda não ideal. 
+          <t xml:space="preserve">Roberto Campos Neto, presidente do Banco Central, revelou que o Pix custa US$ 10 milhões por ano para operar, mas já processa 240 milhões de transações diárias, com custo de desenvolvimento entre US$ 3 e US$ 4 milhões. Ele destacou o sucesso do Pix como porta de entrada para a inovação financeira, junto com Open Finance e Drex (real digital). Campos Neto mencionou o desenvolvimento de agregadores financeiros combinando essas tecnologias e o desafio de escalar o Drex sem comprometer privacidade, programabilidade e descentralização. Soluções em desenvolvimento indicam a viabilidade de aumentar o número de transações em breve. 
 </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>US, O</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>negative (59.90999984741211%)</t>
+          <t>negative (84.12999725341797%)</t>
         </is>
       </c>
     </row>
@@ -579,18 +587,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">O Banco Central (BC) anunciou a abertura de inscrições para a segunda fase do Drex, plataforma de moeda digital, na próxima semana. Com duração de quatro semanas, a chamada visa ampliar a participação do setor privado no projeto, que testará 13 casos de uso de tokenização de ativos, como cessão de recebíveis e crédito colateralizado. O BC espera implementar o novo modelo no início de 2025, com maior participação dos bancos na solução de desafios como a  privacidade das transações. A segurança cibernética e a privacidade são cruciais para o sucesso do projeto, que poderá ser expandido para testes com a população após a validação dessa fase. 
+          <t xml:space="preserve">O Banco Central (BC) abrirá nova chamada para participantes do projeto piloto Drex na próxima semana, com duração mínima de quatro semanas. A iniciativa busca criar uma infraestrutura tokenizada para o sistema financeiro, registrando em blockchain a moeda brasileira e ativos financeiros. O objetivo é testar a  eficiência da tokenização em 13 casos de uso, com maior participação dos bancos na resolução de desafios. Segurança cibernética e privacidade são cruciais para o sucesso do projeto, que poderá ser expandido para a população após testes. Atualmente, 16 consórcios, incluindo grandes bancos, fintechs e empresas de tecnologia, participam do Drex. 
 </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A, O, BC</t>
+          <t xml:space="preserve">- BBAS3
+- BBDC4
+- ITUB4
+- SANB11
+- ABCB4
+- BBDC4
+- BIDI11
+- BPAC11
+- NUBR33 
+- XPBR31
+</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>negative (56.709999084472656%)</t>
+          <t>positive (83.80000305175781%)</t>
         </is>
       </c>
     </row>
@@ -602,18 +620,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">O Banco BV inaugurou filial em Luxemburgo para expandir internacionalmente seus negócios no segmento de atacado.  Com equipe de 10 pessoas, a filial oferecerá produtos como trade finance, empréstimos internacionais e investimentos para clientes corporativos. A iniciativa visa ampliar alternativas de financiamento externo e centralizar as operações em moeda estrangeira, tornando o banco mais competitivo. No primeiro semestre, a carteira de crédito do BV totalizou R$ 88,1 bilhões, com R$ 25,6 bilhões provenientes do atacado. 
+          <t xml:space="preserve">O Banco BV inaugurou uma filial em Luxemburgo com o objetivo de ampliar sua atuação no mercado internacional e oferecer mais opções de financiamento aos clientes corporativos. Com dez funcionários, a unidade fornecerá produtos financeiros como trade finance, empréstimos internacionais e investimentos. A iniciativa visa aumentar a competitividade do banco e centralizar as operações em moeda estrangeira. O BV, que tem o Grupo Votorantim e o Banco do Brasil como sócios, busca expandir sua carteira de crédito, que no primeiro semestre era de R$ 88,1 bilhões, incluindo R$ 25,6 bilhões do segmento atacado. 
 </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A, O, R, BV</t>
+          <t xml:space="preserve">- BBAS3 
+</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>negative (86.88999938964844%)</t>
+          <t>negative (93.62000274658203%)</t>
         </is>
       </c>
     </row>
@@ -625,18 +644,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">O Banco BV inaugurou uma filial em Luxemburgo, visando clientes corporativos e de atacado. Com equipe de dez pessoas, a unidade focará em soluções de trade finance, empréstimos internacionais e produtos de investimento. A iniciativa busca oferecer preços mais competitivos e fortalecer a atuação do BV no mercado financeiro global. 
+          <t xml:space="preserve">O Banco BV inaugurou uma filial em Luxemburgo, visando clientes corporativos e de banco de investimento. Com foco em trade finance, empréstimos internacionais e investimentos, o escritório terá dez funcionários e oferecerá soluções a preços competitivos no mercado financeiro global. A iniciativa reforça a presença do BV em um dos principais centros financeiros do mundo. 
 </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A, O, BV</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>negative (87.62999725341797%)</t>
+          <t>negative (81.30999755859375%)</t>
         </is>
       </c>
     </row>
@@ -648,18 +668,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">O Ibovespa fechou em alta pelo segundo dia, mas enfrenta resistência.  Após bater máxima histórica em agosto, iniciou correção. Se romper suporte em 133.110 pontos, pode cair para 130.400. Rompendo resistência em 134.355 pontos, mira 137.469. Mini-índice acompanha o índice, com suportes e resistências semelhantes. Minidólar fechou em alta, buscando romper resistência em 5.465 pontos. Agenda inclui dados de emprego nos EUA e indicadores de serviços. Mercados internacionais operam em queda, com exceção da bolsa japonesa e petróleo em alta. 
+          <t xml:space="preserve">O Ibovespa fechou em alta pelo segundo dia, mas enfrenta resistência em 134.355/135.200 pontos. Superando essa faixa, pode buscar 136.000/136.840 pontos. Caso contrário, a quebra do suporte em 133.110/132.495 pode levar a 131.815/131.490. Mini-índice fechou em alta, mas precisa superar 134.490/134.785 para continuar subindo. Mini-dólar também subiu e rompe resistência em 5.465/5.478,5 para seguir em alta. Agenda inclui dados de emprego nos EUA e indicadores de serviços. Mercados internacionais operam em queda, com exceção da bolsa japonesa. 
 </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>O, EUA</t>
+          <t xml:space="preserve">- WINV24
+- WDOX24 
+</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>neutral (96.08000183105469%)</t>
+          <t>neutral (96.61000061035156%)</t>
         </is>
       </c>
     </row>
@@ -671,18 +693,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">O mercado financeiro brasileiro reagiu com cautela ao aumento da nota de crédito do Brasil pela Moody's, reconhecendo o cenário desafiador. Roberto Campos Neto, presidente do Banco Central, discursa sobre o tema em dois eventos. Especialistas apontam que a trajetória para o grau de investimento exige controle de gastos. Enquanto isso, a tensão no Oriente Médio e os dados de emprego nos EUA geram cautela. No cenário corporativo, Petrobras, Vale, Gerdau e Ambev tiveram suas notas elevadas. A Vale e o BNDES anunciaram um fundo de investimento em minerais críticos. As eleições municipais entram em seus momentos finais com o último debate em São Paulo.  
+          <t xml:space="preserve">A Moody's elevou a nota de crédito do Brasil, impulsionando o otimismo do mercado, apesar do cenário ainda desafiador. Roberto Campos Neto, presidente do BC, discutirá o impacto da decisão em eventos hoje, defendendo uma taxa de juros neutra menor para o Brasil. A agenda inclui ainda dados econômicos como pedidos de seguro-desemprego nos EUA e resultados do Tesouro Nacional. No cenário internacional, as tensões no Oriente Médio preocupam investidores. As eleições municipais entram em reta final com último debate em SP. Por fim, o governo discute regulamentação das apostas esportivas e a Vale anuncia fundo para minerais críticos com o BNDES. 
 </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>A, O, EUA, BNDES</t>
+          <t xml:space="preserve">- PETR4 
+- VALE3 
+- GGBR4 
+- ABEV3 
+</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>positive (72.66999816894531%)</t>
+          <t>positive (85.56999969482422%)</t>
         </is>
       </c>
     </row>
@@ -694,18 +720,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve">A Moody's manteve o rating da Petrobras em "Ba1", mas elevou sua perspectiva para positiva, refletindo a visão otimista sobre o rating soberano do Brasil e a expectativa de estabilidade no perfil de crédito da estatal. A agência reconhece a baixa probabilidade de default da Petrobras, mesmo sendo uma empresa estatal, devido à solidez de seus indicadores financeiros. A Moody's destaca, porém, a exposição da companhia a mudanças políticas e interferências governamentais como fatores que limitam um rating ainda melhor. 
+          <t xml:space="preserve">A Moody's manteve o rating da Petrobras em "Ba1", mas elevou sua perspectiva para positiva, impulsionada pela perspectiva positiva da nota soberana do Brasil. A agência espera que o perfil de crédito da estatal permaneça estável, com baixo risco de default, devido às suas fortes métricas financeiras. A Moody's reconhece a baixa probabilidade da Petrobras ser afetada por dificuldades de crédito do governo, mas limita o rating devido à potencial influência política nas decisões da empresa. A avaliação positiva reflete a confiança na capacidade da Petrobras de navegar no cenário atual. 
 </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">- PETR3
+- PETR4 
+</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>negative (86.69999694824219%)</t>
+          <t>negative (91.75%)</t>
         </is>
       </c>
     </row>
@@ -717,18 +745,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Diretores financeiros no Brasil planejam usar "títulos verdes" como estratégia ESG para captar recursos. Emissão de "green bonds" e "sustainability bonds" é a segunda maior prioridade, à frente de investimentos em economia circular e energia limpa, segundo pesquisa do Insper e Assetz. Natura e Eletrobras são exemplos de empresas que captaram recursos via títulos verdes recentemente. Apesar da crescente preocupação com ESG, o mercado brasileiro ainda precisa amadurecer nesse quesito. A implementação de normas internacionais de sustentabilidade deve impulsionar a adoção de práticas ESG e fortalecer o mercado de títulos verdes no país. 
+          <t xml:space="preserve">CFOs no Brasil estão priorizando a emissão de títulos verdes, como "green bonds" e "sustainability bonds", como parte de suas estratégias ESG. A emissão desses títulos é vista como a segunda maior prioridade para os próximos anos, superando investimentos em economia circular e energia limpa. Empresas como a Energisa e a Natura já realizaram emissões, destinando os recursos para projetos sustentáveis e desenvolvimento de bioingredientes. Apesar da crescente preocupação com ESG, o mercado brasileiro ainda busca maturidade nesse tipo de captação, mas a implementação de normas internacionais como IFRS S1 e S2 prometem impulsionar o avanço da estratégia. 
 </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>A, ESG</t>
+          <t xml:space="preserve">- NATU3 
+</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>negative (81.29000091552734%)</t>
+          <t>negative (78.9800033569336%)</t>
         </is>
       </c>
     </row>
@@ -740,18 +769,31 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve">A temporada de resultados do 3º trimestre de 2024 começou! O mercado aguarda ansioso pelos números de empresas como Multiplan (24/10), Suzano (24/10), Vale (24/10) e outras gigantes do Ibovespa. As demonstrações financeiras (DFP e ITR) são obrigatórias e devem ser enviadas à CVM em até 90 dias após o fim do trimestre. Fique atento ao calendário para acompanhar o desempenho das empresas, analisar indicadores e tomar decisões de investimento mais assertivas. 
+          <t xml:space="preserve">A temporada de resultados do 3º trimestre de 2024 (3T24) das empresas listadas no Ibovespa já tem datas. O calendário, disponibilizado pela Quantum Finance, abrange a divulgação dos formulários DFP (Demonstrações Financeiras Padronizadas) e ITR (Informações Trimestrais), documentos obrigatórios para companhias abertas. O cronograma detalhado inclui empresas como Multiplan (24/10), Suzano (24/10), Vale (24/10), Usiminas (25/10), Auren (30/10) e outras, com divulgação até 31/10. A metodologia da Quantum considera os calendários da CVM e a composição mais recente do Ibovespa. 
 </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ITR, DFP, CVM, A, O</t>
+          <t xml:space="preserve">- MULT3
+- SUZB3
+- VALE3
+- USIM5
+- AURE3
+- TRPL4
+- WEGE3
+- ABEV3
+- BBDC3
+- BBDC4
+- CCRO3
+- CRFB3
+- EZTC3 
+</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>positive (95.05999755859375%)</t>
+          <t>positive (95.19000244140625%)</t>
         </is>
       </c>
     </row>
@@ -763,18 +805,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Empresas chinesas investiram mais de US$ 100 bilhões em projetos de energia limpa no exterior desde 2023, segundo a CEF. A China domina a produção de painéis solares, baterias e veículos elétricos, gerando preocupações sobre práticas comerciais desleais. EUA, Canadá e UE implementaram tarifas sobre produtos chineses. Em resposta, empresas chinesas, como BYD e CATL, investem em fábricas no exterior para driblar barreiras comerciais. Estima-se que dois terços da capacidade de tecnologia limpa da China buscarão mercados de exportação até 2030. A China critica as sobretaxas, argumentando que prejudicam o combate às mudanças climáticas e aumentam os custos da transição energética global. 
+          <t xml:space="preserve">Empresas chinesas investiram mais de US$ 100 bilhões em tecnologias de energia limpa no exterior desde o início de 2023, buscando contornar barreiras comerciais e expandir sua presença global. A China domina a produção de painéis solares, baterias de lítio e veículos elétricos, o que tem gerado preocupações sobre práticas comerciais desleais e tarifas de importação impostas por países como EUA e Canadá. A União Europeia também considera medidas semelhantes. A China argumenta que as restrições prejudicam os esforços globais de combate às mudanças climáticas. Especialistas estimam que dois terços da capacidade de tecnologia limpa da China excederão a demanda interna até 2030, intensificando a busca por mercados de exportação. 
 </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>EUA, UE, A, US, BYD, CEF, CATL</t>
+          <t xml:space="preserve">- BYD
+- CATL 
+</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>neutral (89.68000030517578%)</t>
+          <t>positive (54.400001525878906%)</t>
         </is>
       </c>
     </row>
@@ -786,21 +830,39 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Os fundos multimercado estão concentrando seus investimentos nas gigantes da bolsa brasileira, especialmente em empresas do setor de commodities como Vale e Petrobras. Um levantamento da Quantum revela que a Vale foi a ação mais comprada entre janeiro e abril de 2024, com uma média mensal de 708 fundos investindo R$ 4,37 bilhões. 
-A preferência por essas ações se deve à sua alta liquidez, o que facilita a entrada e saída de posições. Além disso, a familiaridade e o volume de negociação dessas empresas tornam o processo de investimento mais ágil. 
-Apesar do perfil conservador, alguns fundos têm diversificado suas carteiras com ações menos tradicionais, como Lojas Renner e Allos, que se mantiveram presentes nos portfólios durante todo o período analisado.
-Especialistas apontam que a dificuldade em construir posições em empresas menores e menos líquidas, como as small caps, contribui para a concentração em ações de grande porte. A demora para montar uma posição em empresas com menor liquidez pode levar de quatro a cinco pregões, impactando a agilidade e a rentabilidade das operações. 
+          <t xml:space="preserve">Fundos multimercado estão preferindo investir em empresas consolidadas na bolsa brasileira, principalmente as ligadas a commodities, como Vale e Petrobras, que lideram o ranking das ações mais compradas entre janeiro de 2019 e abril de 2024. Essa estratégia conservadora, segundo especialistas, se deve à alta liquidez dessas ações, facilitando a entrada e saída dos fundos. 
+No topo da lista de ações mais compradas em 2024 estão Vale, Itaú e Petrobras, refletindo a preferência por empresas com grande volume de negociação. Apesar do perfil conservador, algumas empresas "fora do radar" aparecem no ranking, como Lojas Renner e Allos, demonstrando uma diversificação estratégica dos fundos.
+Especialistas apontam que a liquidez é um fator crucial para essa escolha, já que fundos multimercado precisam de agilidade para montar e desmontar posições. A dificuldade em negociar ações menos líquidas, como as de empresas menores (small caps), também influencia essa preferência. Em resumo, os fundos multimercado demonstram aversão a riscos, priorizando empresas sólidas e com alta liquidez na bolsa brasileira. 
 </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>A, R</t>
+          <t xml:space="preserve">- PETR3
+- PETR4
+- LREN3
+- ALOS3
+- VALE3
+- ITUB4
+- ELET3
+- SUZB3
+- PRIO3
+- BPAC11
+- SBSP3
+- EQTL3
+- RENT3
+- VBBR3
+- BBAS3
+- HAPV3
+- RAIL3
+- GGBR4
+- BBDC4 
+</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>positive (86.7300033569336%)</t>
+          <t>positive (86.25%)</t>
         </is>
       </c>
     </row>
@@ -812,18 +874,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">A prisão da influenciadora Deolane Bezerra reacende o debate sobre o impacto da reputação na carreira. O especialista Marcos Tonin alerta para a fragilidade da imagem pública, especialmente para executivos. Segundo ele, a reputação influencia 60% das decisões de compra e líderes com boa imagem têm 30% mais chances de promoção. Empresas com reputação forte podem cobrar até 10% a mais por seus produtos. Tonin destaca a importância da ética, transparência e responsabilidade na construção de uma imagem positiva, crucial para o sucesso profissional e empresarial. 
+          <t xml:space="preserve">A prisão da influenciadora Deolane Bezerra levanta o debate sobre o impacto da reputação na carreira. Especialistas alertam que a imagem pública é crucial para executivos e influenciadores, impactando decisões de compra e até promoções. Ter boa reputação agrega valor à marca pessoal e profissional, abrindo portas e fortalecendo a imagem da empresa como um todo. A transparência e a responsabilidade são essenciais para construir uma imagem positiva e evitar danos à reputação, especialmente na era digital, onde informações se espalham rapidamente. Cuidar da reputação é essencial para o sucesso profissional a longo prazo. 
 </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>A, O</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>positive (86.31999969482422%)</t>
+          <t>positive (81.5999984741211%)</t>
         </is>
       </c>
     </row>
@@ -835,18 +898,52 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Outubro será um mês de proventos para investidores da B3, com 25 empresas pagando dividendos e JCP. Bancos como Bradesco, Itaú e Banese abrem a agenda no dia 1º. O destaque fica para a JBS, que distribuirá R$ 4,436 bilhões em dividendos no dia 7, com pagamento de R$ 2 por ação. A B3 também paga proventos no dia 7, totalizando R$ 516 milhões. Outros destaques incluem Tim, Alupar e Panatlantica. O calendário completo com datas, valores e tipos de proventos está disponível na notícia. É importante lembrar que dividendos são isentos de IR, enquanto JCP está sujeito à alíquota de 15%.
+          <t xml:space="preserve">O mês das crianças também trará presentes para investidores da bolsa brasileira. Pelo menos 25 empresas distribuirão dividendos e JCP em outubro, com destaque para JBS (R$2 por ação em 07/10) e Banese (até R$1,26 por ação em 01/10). O calendário inclui ainda Bradesco, Itaú, B3 e Tim.  Lembre-se que dividendos são isentos de IR, enquanto JCP está sujeito à alíquota de 15%. A data limite para ter direito aos proventos varia conforme a empresa. Consulte o calendário completo na matéria original para verificar valores, datas e tipos de proventos. Investidores atentos podem aproveitar a "chuva de dividendos" de outubro. 
 </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>B3, R, JBS, JCP, A, IR, O</t>
+          <t xml:space="preserve">- BBDC3
+- BBDC4
+- ITUB3
+- ITSA4
+- BEES3
+- BGIP4
+- BGIP3
+- JBSS3
+- TIMS3
+- ALUP3
+- ALUP4
+- ALUP11
+- PATI3
+- PATI4
+- B3SA3
+- VULC3
+- FLRY3
+- MTRE3
+- RDOR3
+- RPAD5
+- LREN3
+- CSUD3
+- ALOS3
+- SOJA3
+- EVEN3
+- EALT3
+- EALT4
+- KLAS3
+- MULT3
+- TUPY3
+- CURY3
+- IGTI11
+- IGTI3
+- IGTI4 
+</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>positive (94.6500015258789%)</t>
+          <t>positive (95.4000015258789%)</t>
         </is>
       </c>
     </row>
@@ -858,18 +955,19 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve">O fechamento de agências bancárias tradicionais contrasta com a expansão das cooperativas de crédito, como o Sicredi, que cresceu 23,9% em 2023, atingindo R$ 731 bilhões em ativos. O Sicredi abriu agências em 779 municípios, sendo a única instituição financeira presente em mais de 200 deles. Com 8,3 milhões de associados, a cooperativa foca em micro e pequenas empresas, além do agronegócio. Inovação tecnológica, com foco em aplicativos e inteligência artificial, também impulsionam o crescimento, assim como as soluções do Open Finance. O objetivo é alcançar 10 milhões de associados até 2025. 
+          <t xml:space="preserve">O Sicredi cresce no Brasil enquanto bancos tradicionais fecham agências. Com foco em municípios menores, a instituição alcançou R$ 731 bilhões em ativos, um aumento de 23,9% em 2023. O Sicredi abriu agências em 779 cidades nos últimos quatro anos, sendo a única opção em mais de 200 delas. A cooperativa atribui o sucesso à expansão para regiões desatendidas, diversificação de serviços e investimento em tecnologia, como IA e Open Finance. Com 8,3 milhões de associados, o Sicredi mira em 10 milhões até 2025, consolidando sua posição como um dos maiores bancos do país. 
 </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>O, R</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>negative (72.44999694824219%)</t>
+          <t>negative (92.41000366210938%)</t>
         </is>
       </c>
     </row>
@@ -881,18 +979,21 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve">A Linklaters assessorou a Africa Finance Corporation (AFC) em dois acordos com Angola e Zâmbia para o desenvolvimento do Corredor do Lobito, projeto ferroviário que ligará o porto angolano à Zâmbia. A AFC, promotora principal, junto a EUA, UE e outros, construirá 800 km de linha, criando uma rota estratégica para exportações da Zâmbia e Congo. O projeto, avaliado em US$ 3 bilhões, visa transportar minerais essenciais, além de produtos agrícolas, impulsionando o comércio regional e global. A Linklaters, com escritórios em Lisboa e Paris, destacou sua experiência em projetos internacionais de grande escala, compromisso com a África e conhecimento do setor mineiro. Os acordos foram assinados em setembro durante a Assembleia Geral da ONU. 
+          <t xml:space="preserve">A Linklaters assessorou a Africa Finance Corporation (AFC) em dois acordos com Angola e Zâmbia para o desenvolvimento do Corredor do Lobito, ligando o porto angolano à Zâmbia por ferrovia. O projeto, com a participação dos EUA, UE e BAD, inclui 800 km de linha férrea, visando o transporte de minerais, produtos agrícolas e o comércio global. 
+A AFC, promotora principal, terá como parceiros Angola, Zâmbia, EUA, UE e BAD. A iniciativa visa criar uma rota estratégica para exportações da Zâmbia e Congo, gerando US$ 3 bilhões em benefícios e 1.250 empregos. 
+A Linklaters, com escritórios em Lisboa e Paris, liderou a assessoria jurídica, destacando a experiência em projetos de infraestrutura e conhecimento do setor mineiro africano. A assinatura dos acordos ocorreu em 24 de setembro, durante a Assembleia Geral da ONU. 
 </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>EUA, UE, A, US, O, ONU, AFC</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>negative (83.56999969482422%)</t>
+          <t>positive (39.150001525878906%)</t>
         </is>
       </c>
     </row>
@@ -904,18 +1005,19 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve">José Maria Rego, fundador da fintech Raize, assume liderança da área de Consumer Finance do Novo Banco. A nomeação visa impulsionar a transformação e crescimento desta área estratégica, que representa mais de 330 milhões de euros em financiamento anual. Rego, conhecido por sua expertise em fintechs, terá como foco a inovação, a aproximação com o cliente e a otimização do modelo de serviço. A mudança reflete a estratégia do Novo Banco de fortalecer áreas chave com líderes experientes e inovadores. Rego deixou a Raize após a Flexdeal tornar-se acionista majoritária em 2024. 
+          <t xml:space="preserve">O Novo Banco contratou José Maria Rego, ex-CEO da fintech Raize, para liderar a área de Consumer Finance. O objetivo é "transformar" a área, que representa mais de 330 milhões de euros em financiamento anual, tornando-a mais ágil, inovadora e focada no cliente. Rego, conhecido pela sua experiência em fintech, visa aproximar o banco dos clientes através de investimentos em tecnologia e otimização de serviços. A nomeação faz parte de uma reformulação estratégica do Novo Banco iniciada em 2023. 
 </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>positive (75.18000030517578%)</t>
+          <t>positive (63.7400016784668%)</t>
         </is>
       </c>
     </row>
@@ -927,18 +1029,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">José Maria Rego, fundador da Raize, assume liderança da área de crédito ao consumo do Novobanco, que representa €330 milhões em financiamento anual. A mudança, parte de uma reforma estratégica, visa tornar o banco mais ágil e focado no cliente através de tecnologia e inovação. Rego pretende aproximar o banco das necessidades dos clientes. Mark Bourke, CEO do Novobanco, celebra a experiência de Rego e o foco na melhor experiência para o cliente. A nomeação segue a chegada de João Paixão Moreira como administrador comercial em maio, reforçando a estrutura do banco. 
+          <t xml:space="preserve">José Maria Rego, fundador da Raize, assume a liderança da área de consumer finance do Novobanco, após deixar o cargo de CEO da fintech vendida para a Flexdeal. A área, com mais de 330 milhões de euros em financiamento a particulares, é estratégica para o banco em sua transformação digital. Rego terá o desafio de investir em tecnologia e inovação para otimizar o modelo de serviço e aproximar o banco dos clientes. A contratação reforça a estrutura do banco, que recentemente nomeou João Paixão Moreira como administrador comercial de retalho. Mark Bourke, CEO do Novobanco, celebra a experiência de Rego para liderar a área e explorar novas oportunidades de crescimento. 
 </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>A, CEO</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>negative (77.66000366210938%)</t>
+          <t>negative (84.3499984741211%)</t>
         </is>
       </c>
     </row>
@@ -950,18 +1053,19 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Novas regras do open finance facilitam o Pix por aproximação, com lançamento previsto para fevereiro de 2025. O sistema, mais leve e eficiente, impulsionará os pagamentos, segundo o Banco Central. O open finance, que permite o compartilhamento de dados entre instituições, visa aumentar a transparência e competitividade no setor. A ferramenta, que está em consolidação, deve ser impulsionada pela inteligência artificial, proporcionando portabilidade mais fluida.  
+          <t xml:space="preserve">Novas regras do open finance devem facilitar o Pix por aproximação, com lançamento previsto para fevereiro de 2025. O sistema, segundo o Banco Central, será mais leve, eficiente e barato. O open finance, que permite o compartilhamento de dados entre instituições financeiras, visa aumentar a  transparência e a competitividade no setor. A expectativa é que 2024 consolide a ferramenta, impulsionada pela inteligência artificial.  
 </t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>A, O</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>positive (62.56999969482422%)</t>
+          <t>negative (63.119998931884766%)</t>
         </is>
       </c>
     </row>
@@ -973,18 +1077,19 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">O Banco Central prevê que o Pix por aproximação, com lançamento em fevereiro de 2025, terá implementação facilitada pelas novas regras do open finance, lançadas em julho. O sistema, mais leve e eficiente, reduzirá custos para consumidores e lojistas. O open finance, que permite o compartilhamento de dados entre instituições financeiras, visa aumentar a  transparência e a competitividade no setor. Segundo o diretor do BC, Otávio Damaso, 2024 será o ano de consolidação da ferramenta, impulsionada pela inteligência artificial e portabilidades mais fluidas. 
+          <t xml:space="preserve">As novas regras do open finance devem facilitar a implementação do Pix por aproximação, com lançamento previsto para fevereiro de 2025. O novo arcabouço regulatório torna o modelo mais leve, eficiente e barato, tanto para o consumidor quanto para o lojista. O open finance, iniciativa do Banco Central para o compartilhamento de dados, visa aumentar a transparência e competitividade no setor financeiro. A expectativa é que 2024 seja o ano de consolidação da ferramenta, impulsionada pelo uso da inteligência artificial e por portabilidades mais fluidas. 
 </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>O, BC</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>negative (64.37000274658203%)</t>
+          <t>negative (71.16000366210938%)</t>
         </is>
       </c>
     </row>
@@ -996,18 +1101,19 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">O Banco Central prevê que as novas regras do open finance facilitarão a implementação do Pix por aproximação em 2025. O sistema, mais leve e eficiente, reduzirá custos para consumidores e lojistas. O open finance, que visa maior controle do consumidor sobre seus dados, impulsionará a portabilidade de crédito e salários. O desafio é ampliar o uso entre pessoas jurídicas, com foco em casos de uso que facilitem a vida do PJ, inspirados em modelos internacionais como o do Reino Unido.  
+          <t xml:space="preserve">As novas regras do open finance facilitarão o Pix por aproximação, com lançamento em fevereiro de 2025. O sistema, mais leve e eficiente, reduz custos e impulsiona os pagamentos, segundo o Banco Central. A iniciativa visa maior controle do consumidor sobre suas finanças, com comparação de produtos, taxas competitivas e transparência no setor.  Em 2024, o foco é a consolidação da ferramenta, impulsionada pela IA, com funcionalidades para portabilidade de crédito e salários. O desafio é ampliar o uso entre pessoas jurídicas, explorando casos de uso e aprendendo com experiências internacionais, como a do Reino Unido. 
 </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>O, PJ</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>positive (60.47999954223633%)</t>
+          <t>positive (68.44999694824219%)</t>
         </is>
       </c>
     </row>
@@ -1019,18 +1125,19 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve">As novas regras do open finance, sistema de compartilhamento de dados do Banco Central, devem facilitar a implementação do Pix por aproximação, com lançamento em fevereiro de 2025. O novo arcabouço regulatório torna o modelo mais eficiente e barato, segundo o diretor do BC, Otávio Damaso. O open finance, que permite o compartilhamento de dados entre instituições financeiras, visa aumentar a  transparência e a competitividade no setor.  Damaso acredita que 2024 será o ano de consolidação da ferramenta, impulsionada pela inteligência artificial, com portabilidades mais fluidas. 
+          <t xml:space="preserve">As novas regras do open finance, sistema de compartilhamento de dados do Banco Central, devem facilitar a implementação do Pix por aproximação, com lançamento previsto para fevereiro de 2025. O novo arcabouço regulatório, lançado em julho, tornará o sistema mais leve, eficiente e barato, segundo o diretor de regulação do BC, Otávio Damaso. O open finance visa aumentar a transparência e a competitividade no setor financeiro, possibilitando melhores condições e personalização de ofertas. A expectativa é que 2024 seja o ano de consolidação da ferramenta, impulsionada pelo uso da inteligência artificial, com portabilidades mais fluidas. 
 </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>O, BC</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>negative (60.720001220703125%)</t>
+          <t>negative (71.7300033569336%)</t>
         </is>
       </c>
     </row>
@@ -1042,18 +1149,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve">As transferências inteligentes, funcionalidade do open finance que permite automatizar envios via Pix entre contas do mesmo usuário, ainda estão em fase inicial de adoção devido a dificuldades técnicas. Fintechs como Mercado Pago e Noh relatam problemas na autorização e efetivação das transações por parte de algumas instituições. Apesar dos obstáculos, a promessa de praticidade e organização financeira tem atraído usuários, que podem, por exemplo, abastecer contas conjuntas ou evitar saldos negativos de forma automática. A expectativa é que, com o tempo, as falhas sejam corrigidas e a funcionalidade se popularize. 
+          <t xml:space="preserve">As transferências inteligentes, funcionalidade do open finance que permite movimentar dinheiro automaticamente entre contas do mesmo titular via Pix, ainda enfrentam obstáculos técnicos. Apesar da promessa de praticidade, com a automatização de pagamentos e consolidação de recursos, a instabilidade nas conexões entre instituições financeiras causa frustração e lentidão. Fintechs como Mercado Pago e Noh relatam dificuldades na autorização e conversão de pagamentos, impactando a experiência do usuário. O Banco Central reconhece os desafios iniciais e trabalha para aprimorar a infraestrutura do sistema, buscando maior estabilidade e agilidade nas transferências.
 </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>neutral (63.20000076293945%)</t>
+          <t>neutral (92.75%)</t>
         </is>
       </c>
     </row>
@@ -1065,20 +1173,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve">A China, famosa por suas megaconstruções, enfrenta um dilema com o Goldin Finance 117, o maior arranha-céu abandonado do mundo. Localizado em Tianjin, o prédio de 597 metros deveria ser o coração de um luxuoso complexo comercial, mas foi atingido por diversos problemas financeiros e pela recessão imobiliária. Iniciado em 2008, o projeto sofreu várias paralisações, deixando a estrutura inacabada, com apenas 3/4 da fachada coberta. 
-O fracasso do Goldin Finance 117 levou o governo chinês a repensar suas políticas de construção. Buscando recuperar a identidade arquitetônica e evitar novas obras faraônicas inacabadas, o governo de Xi Jinping proibiu a construção de prédios com mais de 500 metros de altura. Além disso,  estabeleceu limites para torres acima de 250 metros e impôs rigorosas medidas de segurança para edifícios com mais de 100 metros. 
-O Goldin Finance 117 serve como um lembrete visível dos desafios e excessos da construção desenfreada na China, impactando diretamente as futuras políticas de planejamento urbano do país. 
+          <t xml:space="preserve">O artigo discute a história do Goldin Finance 117, um arranha-céu inacabado na China que se tornou o prédio abandonado mais alto do mundo. Localizado em Tianjin, o projeto ambicioso pretendia ser um marco de 597 metros, parte de um complexo de luxo.
+Iniciado em 2008, o projeto enfrentou múltiplas paralisações devido à recessão no mercado imobiliário chinês. Apesar de ter retomado a construção em diferentes momentos, a obra foi definitivamente interrompida em 2019, com cerca de 3/4 da fachada concluída.
+A incapacidade da construtora de Hong Kong em obter financiamento governamental e a falta de rentabilidade do projeto contribuíram para seu abandono. 
+O fracasso do Goldin Finance 117 levou o governo chinês a implementar novas restrições de altura para edifícios. Agora, estruturas acima de 500 metros são proibidas, enquanto aquelas com mais de 250 metros enfrentam limitações severas. Essa mudança visa recuperar a identidade arquitetônica da China e evitar projetos semelhantes.
 </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>A, O</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>neutral (90.62999725341797%)</t>
+          <t>neutral (95.58000183105469%)</t>
         </is>
       </c>
     </row>
@@ -1090,18 +1200,19 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">A CVM anunciou novas regras para portabilidade de investimentos, com foco em desburocratização,  transparência e segurança. A partir de 1º de julho de 2024,  a Resolução CVM 210 permitirá interface digital para solicitação,  escolha do ponto de solicitação, prazos transparentes, acompanhamento em tempo real e  penalidades para atrasos. A medida visa fortalecer o mercado de capitais, empoderar o investidor e  fomentar a competição. As regras  se integrarão ao Open Finance para maior automatização e  prospecção de clientes. 
+          <t xml:space="preserve">A CVM publicou novas regras para portabilidade de investimentos, com foco na desburocratização e simplificação do processo. A partir de julho de 2024, a  portabilidade poderá ser solicitada digitalmente, com acompanhamento em tempo real e prazos mais transparentes. As instituições financeiras serão responsáveis por auxiliar os investidores durante a migração. A CVM destaca a importância da medida para o Open Finance, que permitirá a consulta automatizada de dados e fomentará a concorrência no mercado de capitais. A autarquia também trabalha na integração da portabilidade de investimentos ao Open Finance, visando maior automatização e melhor experiência para o usuário. 
 </t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>A, CVM</t>
+          <t xml:space="preserve">- N/A 
+</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>positive (76.73999786376953%)</t>
+          <t>positive (75.69000244140625%)</t>
         </is>
       </c>
     </row>

</xml_diff>